<commit_message>
made som overall changes in the code, comment and rapport
</commit_message>
<xml_diff>
--- a/rapport/ERdiagram.xlsx
+++ b/rapport/ERdiagram.xlsx
@@ -42,9 +42,6 @@
     <t>fremmenøgle</t>
   </si>
   <si>
-    <t>tabelnavn</t>
-  </si>
-  <si>
     <t>atributter</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>sælgerspil_ID</t>
+  </si>
+  <si>
+    <t>Entitetsklasse</t>
   </si>
 </sst>
 </file>
@@ -402,26 +402,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -865,8 +865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -892,7 +892,7 @@
       <c r="A4" s="1"/>
       <c r="C4" s="3"/>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
@@ -918,23 +918,23 @@
     <row r="8" spans="1:12" ht="15.75" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="14"/>
-      <c r="C8" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
+      <c r="C8" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
       <c r="F8" s="11"/>
       <c r="G8" s="7" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" thickBot="1">
       <c r="A9" s="1"/>
       <c r="B9" s="14"/>
-      <c r="C9" s="29"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="31"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="32"/>
       <c r="F9" s="11"/>
       <c r="G9" s="4" t="s">
         <v>4</v>
@@ -961,13 +961,13 @@
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:12">
       <c r="B12" s="14"/>
-      <c r="C12" s="32"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="11"/>
       <c r="E12" s="11"/>
       <c r="F12" s="11"/>
@@ -986,15 +986,15 @@
     <row r="14" spans="1:12" ht="20.25" customHeight="1">
       <c r="B14" s="14"/>
       <c r="C14" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="11"/>
       <c r="E14" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" s="12"/>
     </row>
@@ -1007,13 +1007,13 @@
         <v>1</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F15" s="15">
         <v>1</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="12"/>
     </row>
@@ -1023,16 +1023,16 @@
         <v>0</v>
       </c>
       <c r="D16" s="16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>5</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H16" s="12"/>
     </row>
@@ -1043,13 +1043,13 @@
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H17" s="12"/>
     </row>
@@ -1060,11 +1060,11 @@
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H18" s="12"/>
     </row>
@@ -1075,7 +1075,7 @@
       </c>
       <c r="D19" s="11"/>
       <c r="E19" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F19" s="11"/>
       <c r="G19" s="24"/>
@@ -1088,7 +1088,7 @@
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F20" s="11"/>
       <c r="G20" s="24"/>

</xml_diff>